<commit_message>
Version 0.8.3 - FIXED changed descriptor to add maven profiles support, mainly added platform for dependency and added os/platform etc to property - FIXED NutsFormat now creates any missing parent folders when calling print(Path/File) or println(Path/File) - CHANGED removed deprecated feature inheritedLog - CHANGED removed deprecated ClassifierMapping
</commit_message>
<xml_diff>
--- a/DEV_VERSION_TRACKING.xlsx
+++ b/DEV_VERSION_TRACKING.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="24375" windowHeight="11895" tabRatio="500"/>
+    <workbookView windowWidth="27975" windowHeight="13005" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
   <si>
     <t>Nuts projects versions Tracking</t>
   </si>
@@ -83,7 +83,7 @@
     <t>0.8.2.1</t>
   </si>
   <si>
-    <t>0.8.2.2</t>
+    <t>0.8.3.0</t>
   </si>
   <si>
     <t>nclown</t>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>nsh</t>
+  </si>
+  <si>
+    <t>fixed echo NTF</t>
   </si>
   <si>
     <t>Ntalk-agent</t>
@@ -149,12 +152,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -192,6 +195,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,8 +233,98 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,134 +345,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +361,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF2A6099"/>
         <bgColor rgb="FF666699"/>
       </patternFill>
@@ -387,31 +397,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6D6D"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFD7D7"/>
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,13 +553,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,145 +565,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,17 +612,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,6 +632,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,26 +660,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,15 +692,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -705,145 +700,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
@@ -856,12 +860,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1252,8 +1257,8 @@
   <sheetPr/>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5333333333333" defaultRowHeight="12.75"/>
@@ -1274,7 +1279,7 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
@@ -1285,7 +1290,7 @@
       <c r="A2" s="2">
         <v>44444</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="I2" t="s">
@@ -1293,7 +1298,7 @@
       </c>
     </row>
     <row r="3" spans="8:9">
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="I3" t="s">
@@ -1313,7 +1318,7 @@
       <c r="F4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I4" t="s">
@@ -1333,7 +1338,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="I5" t="s">
@@ -1347,16 +1352,16 @@
       <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1367,16 +1372,16 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1387,10 +1392,10 @@
       <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -1410,10 +1415,10 @@
       <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1422,7 +1427,7 @@
       <c r="F9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1433,10 +1438,10 @@
       <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1445,7 +1450,7 @@
       <c r="F10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1456,10 +1461,10 @@
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="C11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -1468,7 +1473,7 @@
       <c r="F11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1479,10 +1484,10 @@
       <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -1491,7 +1496,7 @@
       <c r="F12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1502,10 +1507,10 @@
       <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -1514,7 +1519,7 @@
       <c r="F13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1525,10 +1530,10 @@
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -1537,7 +1542,7 @@
       <c r="F14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1548,10 +1553,10 @@
       <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -1560,7 +1565,7 @@
       <c r="F15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1571,10 +1576,10 @@
       <c r="B16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -1583,7 +1588,7 @@
       <c r="F16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1594,10 +1599,10 @@
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="C17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1606,7 +1611,7 @@
       <c r="F17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1617,10 +1622,10 @@
       <c r="B18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="C18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -1629,7 +1634,7 @@
       <c r="F18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1640,31 +1645,33 @@
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="14"/>
+      <c r="E19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" ht="15" spans="1:7">
       <c r="A20" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -1673,21 +1680,21 @@
       <c r="F20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -1696,21 +1703,21 @@
       <c r="F21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="7" t="s">
@@ -1719,21 +1726,21 @@
       <c r="F22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:7">
       <c r="A23" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="C23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -1742,21 +1749,21 @@
       <c r="F23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:7">
       <c r="A24" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="7" t="s">
@@ -1765,7 +1772,7 @@
       <c r="F24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="15" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>